<commit_message>
2025 World Cup ITA
</commit_message>
<xml_diff>
--- a/2025 Junior Pan Am Games Ranking.xlsx
+++ b/2025 Junior Pan Am Games Ranking.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trevorstirling/Library/CloudStorage/Dropbox/Documents/Trampoline/Websites/Trampoline Canada Website/Ranking Lists/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7849F2F3-116E-C74F-980A-D4E35150D748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{709BBE27-8395-FA4D-9FB7-415AA4202B5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="1320" windowWidth="27640" windowHeight="16940" xr2:uid="{9735B40D-4AEE-5E4C-91A9-D577A1054C8F}"/>
   </bookViews>
@@ -17,8 +17,8 @@
     <sheet name="TRA-W" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'TRA-M'!$A$1:$T$2</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'TRA-W'!$A$1:$T$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'TRA-M'!$A$1:$V$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'TRA-W'!$A$1:$V$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="38">
   <si>
     <t>Rank</t>
   </si>
@@ -174,6 +174,9 @@
   </si>
   <si>
     <t>NOSSACK, Sophie</t>
+  </si>
+  <si>
+    <t>Semifinal</t>
   </si>
 </sst>
 </file>
@@ -271,24 +274,6 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -304,11 +289,70 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B0F0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF002060"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF7030A0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE6C6FB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -638,7 +682,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58EF7559-DEC1-374C-BE9A-EB931A8A53CD}">
-  <dimension ref="A1:S19"/>
+  <dimension ref="A1:U19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:A2"/>
@@ -651,61 +695,63 @@
     <col min="7" max="7" width="15.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.83203125" style="4"/>
     <col min="13" max="13" width="10.83203125" style="4"/>
-    <col min="16" max="16" width="10.83203125" style="4"/>
-    <col min="19" max="19" width="10.83203125" style="4"/>
+    <col min="17" max="17" width="10.83203125" style="4"/>
+    <col min="21" max="21" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="14"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="13" t="s">
+      <c r="I1" s="8"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="14"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="13" t="s">
+      <c r="L1" s="8"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="14"/>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="R1" s="14"/>
-      <c r="S1" s="15"/>
-    </row>
-    <row r="2" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="10"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="9"/>
+    </row>
+    <row r="2" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="13"/>
       <c r="H2" s="1" t="s">
         <v>9</v>
       </c>
@@ -730,20 +776,26 @@
       <c r="O2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="P2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="T2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="U2" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A3" cm="1">
         <f t="array" ref="A3">IF(C3="P",SUMPRODUCT(--(D$3:D$82&gt;D3),--(C$3:C$82="P"))+1,"")</f>
         <v>1</v>
@@ -755,19 +807,19 @@
         <v>4</v>
       </c>
       <c r="D3" s="5">
-        <f t="shared" ref="D3:D19" si="0">SUM(E3:G3)</f>
+        <f>SUM(E3:G3)</f>
         <v>109.33</v>
       </c>
       <c r="E3" s="5">
-        <f t="shared" ref="E3:E19" si="1">MAX(H3:M3)</f>
+        <f>MAX(H3:M3)</f>
         <v>54.92</v>
       </c>
       <c r="F3" s="5">
-        <f t="shared" ref="F3:F19" si="2">IF(COUNT(H3:M3)&gt;1,LARGE(H3:M3,2),0)</f>
+        <f>IF(COUNT(H3:M3)&gt;1,LARGE(H3:M3,2),0)</f>
         <v>54.41</v>
       </c>
       <c r="G3" s="6">
-        <f t="shared" ref="G3:G19" si="3">IF(MAX(N3:S3)-F3&gt;0,MAX(N3:S3)-F3,0)</f>
+        <f>IF(MAX(N3:U3)-F3&gt;0,MAX(N3:U3)-F3,0)</f>
         <v>0</v>
       </c>
       <c r="H3" s="5">
@@ -784,12 +836,14 @@
       <c r="M3" s="6"/>
       <c r="N3" s="5"/>
       <c r="O3" s="5"/>
-      <c r="P3" s="6"/>
-      <c r="Q3" s="5"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="6"/>
       <c r="R3" s="5"/>
-      <c r="S3" s="6"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="S3" s="5"/>
+      <c r="T3" s="5"/>
+      <c r="U3" s="6"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" cm="1">
         <f t="array" ref="A4">IF(C4="P",SUMPRODUCT(--(D$3:D$82&gt;D4),--(C$3:C$82="P"))+1,"")</f>
         <v>2</v>
@@ -801,20 +855,20 @@
         <v>4</v>
       </c>
       <c r="D4" s="5">
-        <f t="shared" si="0"/>
-        <v>106.57999999999998</v>
+        <f>SUM(E4:G4)</f>
+        <v>107.85999999999999</v>
       </c>
       <c r="E4" s="5">
-        <f t="shared" si="1"/>
+        <f>MAX(H4:M4)</f>
         <v>54.589999999999996</v>
       </c>
       <c r="F4" s="5">
-        <f t="shared" si="2"/>
+        <f>IF(COUNT(H4:M4)&gt;1,LARGE(H4:M4,2),0)</f>
         <v>51.989999999999995</v>
       </c>
       <c r="G4" s="6">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f>IF(MAX(N4:U4)-F4&gt;0,MAX(N4:U4)-F4,0)</f>
+        <v>1.2800000000000011</v>
       </c>
       <c r="H4" s="5">
         <v>48.71</v>
@@ -828,14 +882,20 @@
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
       <c r="M4" s="6"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
-      <c r="P4" s="6"/>
-      <c r="Q4" s="5"/>
+      <c r="N4" s="5">
+        <v>53.269999999999996</v>
+      </c>
+      <c r="O4" s="5">
+        <v>11.32</v>
+      </c>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="6"/>
       <c r="R4" s="5"/>
-      <c r="S4" s="6"/>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="S4" s="5"/>
+      <c r="T4" s="5"/>
+      <c r="U4" s="6"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" cm="1">
         <f t="array" ref="A5">IF(C5="P",SUMPRODUCT(--(D$3:D$82&gt;D5),--(C$3:C$82="P"))+1,"")</f>
         <v>3</v>
@@ -847,19 +907,19 @@
         <v>4</v>
       </c>
       <c r="D5" s="5">
-        <f t="shared" si="0"/>
+        <f>SUM(E5:G5)</f>
         <v>105.11</v>
       </c>
       <c r="E5" s="5">
-        <f t="shared" si="1"/>
+        <f>MAX(H5:M5)</f>
         <v>54.74</v>
       </c>
       <c r="F5" s="5">
-        <f t="shared" si="2"/>
+        <f>IF(COUNT(H5:M5)&gt;1,LARGE(H5:M5,2),0)</f>
         <v>50.37</v>
       </c>
       <c r="G5" s="6">
-        <f t="shared" si="3"/>
+        <f>IF(MAX(N5:U5)-F5&gt;0,MAX(N5:U5)-F5,0)</f>
         <v>0</v>
       </c>
       <c r="H5" s="5">
@@ -876,12 +936,14 @@
       <c r="M5" s="6"/>
       <c r="N5" s="5"/>
       <c r="O5" s="5"/>
-      <c r="P5" s="6"/>
-      <c r="Q5" s="5"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="6"/>
       <c r="R5" s="5"/>
-      <c r="S5" s="6"/>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="S5" s="5"/>
+      <c r="T5" s="5"/>
+      <c r="U5" s="6"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" t="str" cm="1">
         <f t="array" ref="A6">IF(C6="P",SUMPRODUCT(--(D$3:D$82&gt;D6),--(C$3:C$82="P"))+1,"")</f>
         <v/>
@@ -891,19 +953,19 @@
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="5">
-        <f t="shared" si="0"/>
+        <f>SUM(E6:G6)</f>
         <v>105.00999999999999</v>
       </c>
       <c r="E6" s="5">
-        <f t="shared" si="1"/>
+        <f>MAX(H6:M6)</f>
         <v>54.45</v>
       </c>
       <c r="F6" s="5">
-        <f t="shared" si="2"/>
+        <f>IF(COUNT(H6:M6)&gt;1,LARGE(H6:M6,2),0)</f>
         <v>50.559999999999995</v>
       </c>
       <c r="G6" s="6">
-        <f t="shared" si="3"/>
+        <f>IF(MAX(N6:U6)-F6&gt;0,MAX(N6:U6)-F6,0)</f>
         <v>0</v>
       </c>
       <c r="H6" s="5">
@@ -920,12 +982,14 @@
       <c r="M6" s="6"/>
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
-      <c r="P6" s="6"/>
-      <c r="Q6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="6"/>
       <c r="R6" s="5"/>
-      <c r="S6" s="6"/>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="S6" s="5"/>
+      <c r="T6" s="5"/>
+      <c r="U6" s="6"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" t="str" cm="1">
         <f t="array" ref="A7">IF(C7="P",SUMPRODUCT(--(D$3:D$82&gt;D7),--(C$3:C$82="P"))+1,"")</f>
         <v/>
@@ -935,19 +999,19 @@
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="5">
-        <f t="shared" si="0"/>
+        <f>SUM(E7:G7)</f>
         <v>104.88</v>
       </c>
       <c r="E7" s="5">
-        <f t="shared" si="1"/>
+        <f>MAX(H7:M7)</f>
         <v>53.91</v>
       </c>
       <c r="F7" s="5">
-        <f t="shared" si="2"/>
+        <f>IF(COUNT(H7:M7)&gt;1,LARGE(H7:M7,2),0)</f>
         <v>50.97</v>
       </c>
       <c r="G7" s="6">
-        <f t="shared" si="3"/>
+        <f>IF(MAX(N7:U7)-F7&gt;0,MAX(N7:U7)-F7,0)</f>
         <v>0</v>
       </c>
       <c r="H7" s="5">
@@ -964,12 +1028,14 @@
       <c r="M7" s="6"/>
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
-      <c r="P7" s="6"/>
-      <c r="Q7" s="5"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="6"/>
       <c r="R7" s="5"/>
-      <c r="S7" s="6"/>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="S7" s="5"/>
+      <c r="T7" s="5"/>
+      <c r="U7" s="6"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" t="str" cm="1">
         <f t="array" ref="A8">IF(C8="P",SUMPRODUCT(--(D$3:D$82&gt;D8),--(C$3:C$82="P"))+1,"")</f>
         <v/>
@@ -979,19 +1045,19 @@
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="5">
-        <f t="shared" si="0"/>
+        <f>SUM(E8:G8)</f>
         <v>102.61</v>
       </c>
       <c r="E8" s="5">
-        <f t="shared" si="1"/>
+        <f>MAX(H8:M8)</f>
         <v>51.33</v>
       </c>
       <c r="F8" s="5">
-        <f t="shared" si="2"/>
+        <f>IF(COUNT(H8:M8)&gt;1,LARGE(H8:M8,2),0)</f>
         <v>51.28</v>
       </c>
       <c r="G8" s="6">
-        <f t="shared" si="3"/>
+        <f>IF(MAX(N8:U8)-F8&gt;0,MAX(N8:U8)-F8,0)</f>
         <v>0</v>
       </c>
       <c r="H8" s="5">
@@ -1008,12 +1074,14 @@
       <c r="M8" s="6"/>
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
-      <c r="P8" s="6"/>
-      <c r="Q8" s="5"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="6"/>
       <c r="R8" s="5"/>
-      <c r="S8" s="6"/>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="S8" s="5"/>
+      <c r="T8" s="5"/>
+      <c r="U8" s="6"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" t="str" cm="1">
         <f t="array" ref="A9">IF(C9="P",SUMPRODUCT(--(D$3:D$82&gt;D9),--(C$3:C$82="P"))+1,"")</f>
         <v/>
@@ -1023,19 +1091,19 @@
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="5">
-        <f t="shared" si="0"/>
+        <f>SUM(E9:G9)</f>
         <v>100.28</v>
       </c>
       <c r="E9" s="5">
-        <f t="shared" si="1"/>
+        <f>MAX(H9:M9)</f>
         <v>52.05</v>
       </c>
       <c r="F9" s="5">
-        <f t="shared" si="2"/>
+        <f>IF(COUNT(H9:M9)&gt;1,LARGE(H9:M9,2),0)</f>
         <v>48.230000000000004</v>
       </c>
       <c r="G9" s="6">
-        <f t="shared" si="3"/>
+        <f>IF(MAX(N9:U9)-F9&gt;0,MAX(N9:U9)-F9,0)</f>
         <v>0</v>
       </c>
       <c r="H9" s="5">
@@ -1052,12 +1120,14 @@
       <c r="M9" s="6"/>
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
-      <c r="P9" s="6"/>
-      <c r="Q9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="6"/>
       <c r="R9" s="5"/>
-      <c r="S9" s="6"/>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="S9" s="5"/>
+      <c r="T9" s="5"/>
+      <c r="U9" s="6"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" cm="1">
         <f t="array" ref="A10">IF(C10="P",SUMPRODUCT(--(D$3:D$82&gt;D10),--(C$3:C$82="P"))+1,"")</f>
         <v>4</v>
@@ -1069,19 +1139,19 @@
         <v>4</v>
       </c>
       <c r="D10" s="5">
-        <f t="shared" si="0"/>
+        <f>SUM(E10:G10)</f>
         <v>99.32</v>
       </c>
       <c r="E10" s="5">
-        <f t="shared" si="1"/>
+        <f>MAX(H10:M10)</f>
         <v>51.749999999999993</v>
       </c>
       <c r="F10" s="5">
-        <f t="shared" si="2"/>
+        <f>IF(COUNT(H10:M10)&gt;1,LARGE(H10:M10,2),0)</f>
         <v>47.57</v>
       </c>
       <c r="G10" s="6">
-        <f t="shared" si="3"/>
+        <f>IF(MAX(N10:U10)-F10&gt;0,MAX(N10:U10)-F10,0)</f>
         <v>0</v>
       </c>
       <c r="H10" s="5">
@@ -1098,12 +1168,14 @@
       <c r="M10" s="6"/>
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
-      <c r="P10" s="6"/>
-      <c r="Q10" s="5"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="6"/>
       <c r="R10" s="5"/>
-      <c r="S10" s="6"/>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="S10" s="5"/>
+      <c r="T10" s="5"/>
+      <c r="U10" s="6"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" t="str" cm="1">
         <f t="array" ref="A11">IF(C11="P",SUMPRODUCT(--(D$3:D$82&gt;D11),--(C$3:C$82="P"))+1,"")</f>
         <v/>
@@ -1113,19 +1185,19 @@
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="5">
-        <f t="shared" si="0"/>
+        <f>SUM(E11:G11)</f>
         <v>97.859999999999985</v>
       </c>
       <c r="E11" s="5">
-        <f t="shared" si="1"/>
+        <f>MAX(H11:M11)</f>
         <v>48.949999999999996</v>
       </c>
       <c r="F11" s="5">
-        <f t="shared" si="2"/>
+        <f>IF(COUNT(H11:M11)&gt;1,LARGE(H11:M11,2),0)</f>
         <v>48.91</v>
       </c>
       <c r="G11" s="6">
-        <f t="shared" si="3"/>
+        <f>IF(MAX(N11:U11)-F11&gt;0,MAX(N11:U11)-F11,0)</f>
         <v>0</v>
       </c>
       <c r="H11" s="5">
@@ -1142,12 +1214,14 @@
       <c r="M11" s="6"/>
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
-      <c r="P11" s="6"/>
-      <c r="Q11" s="5"/>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="6"/>
       <c r="R11" s="5"/>
-      <c r="S11" s="6"/>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="S11" s="5"/>
+      <c r="T11" s="5"/>
+      <c r="U11" s="6"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" t="str" cm="1">
         <f t="array" ref="A12">IF(C12="P",SUMPRODUCT(--(D$3:D$82&gt;D12),--(C$3:C$82="P"))+1,"")</f>
         <v/>
@@ -1157,19 +1231,19 @@
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="5">
-        <f t="shared" si="0"/>
+        <f>SUM(E12:G12)</f>
         <v>92.04</v>
       </c>
       <c r="E12" s="5">
-        <f t="shared" si="1"/>
+        <f>MAX(H12:M12)</f>
         <v>48.080000000000005</v>
       </c>
       <c r="F12" s="5">
-        <f t="shared" si="2"/>
+        <f>IF(COUNT(H12:M12)&gt;1,LARGE(H12:M12,2),0)</f>
         <v>43.96</v>
       </c>
       <c r="G12" s="6">
-        <f t="shared" si="3"/>
+        <f>IF(MAX(N12:U12)-F12&gt;0,MAX(N12:U12)-F12,0)</f>
         <v>0</v>
       </c>
       <c r="H12" s="5">
@@ -1186,217 +1260,233 @@
       <c r="M12" s="6"/>
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
-      <c r="P12" s="6"/>
-      <c r="Q12" s="5"/>
+      <c r="P12" s="5"/>
+      <c r="Q12" s="6"/>
       <c r="R12" s="5"/>
-      <c r="S12" s="6"/>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="S12" s="5"/>
+      <c r="T12" s="5"/>
+      <c r="U12" s="6"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" cm="1">
         <f t="array" ref="A13">IF(C13="P",SUMPRODUCT(--(D$3:D$82&gt;D13),--(C$3:C$82="P"))+1,"")</f>
         <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D13" s="5">
-        <f t="shared" si="0"/>
-        <v>82.51</v>
+        <f>SUM(E13:G13)</f>
+        <v>88.72</v>
       </c>
       <c r="E13" s="5">
-        <f t="shared" si="1"/>
-        <v>55.410000000000004</v>
+        <f>MAX(H13:M13)</f>
+        <v>35.85</v>
       </c>
       <c r="F13" s="5">
-        <f t="shared" si="2"/>
-        <v>27.099999999999998</v>
+        <f>IF(COUNT(H13:M13)&gt;1,LARGE(H13:M13,2),0)</f>
+        <v>6.3199999999999994</v>
       </c>
       <c r="G13" s="6">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f>IF(MAX(N13:U13)-F13&gt;0,MAX(N13:U13)-F13,0)</f>
+        <v>46.55</v>
       </c>
       <c r="H13" s="5">
-        <v>55.410000000000004</v>
+        <v>6.3199999999999994</v>
       </c>
       <c r="I13" s="5">
-        <v>6.27</v>
-      </c>
-      <c r="J13" s="6">
-        <v>27.099999999999998</v>
-      </c>
+        <v>35.85</v>
+      </c>
+      <c r="J13" s="6"/>
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
       <c r="M13" s="6"/>
-      <c r="N13" s="5"/>
-      <c r="O13" s="5"/>
-      <c r="P13" s="6"/>
-      <c r="Q13" s="5"/>
+      <c r="N13" s="5">
+        <v>52.87</v>
+      </c>
+      <c r="O13" s="5">
+        <v>52.25</v>
+      </c>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="6"/>
       <c r="R13" s="5"/>
-      <c r="S13" s="6"/>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A14" t="str" cm="1">
+      <c r="S13" s="5"/>
+      <c r="T13" s="5"/>
+      <c r="U13" s="6"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A14" cm="1">
         <f t="array" ref="A14">IF(C14="P",SUMPRODUCT(--(D$3:D$82&gt;D14),--(C$3:C$82="P"))+1,"")</f>
-        <v/>
+        <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="3"/>
+        <v>17</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>4</v>
+      </c>
       <c r="D14" s="5">
-        <f t="shared" si="0"/>
-        <v>79.69</v>
+        <f>SUM(E14:G14)</f>
+        <v>82.51</v>
       </c>
       <c r="E14" s="5">
-        <f t="shared" si="1"/>
-        <v>50.71</v>
+        <f>MAX(H14:M14)</f>
+        <v>55.410000000000004</v>
       </c>
       <c r="F14" s="5">
-        <f t="shared" si="2"/>
-        <v>28.979999999999997</v>
+        <f>IF(COUNT(H14:M14)&gt;1,LARGE(H14:M14,2),0)</f>
+        <v>27.099999999999998</v>
       </c>
       <c r="G14" s="6">
-        <f t="shared" si="3"/>
+        <f>IF(MAX(N14:U14)-F14&gt;0,MAX(N14:U14)-F14,0)</f>
         <v>0</v>
       </c>
       <c r="H14" s="5">
-        <v>50.71</v>
+        <v>55.410000000000004</v>
       </c>
       <c r="I14" s="5">
-        <v>17.73</v>
+        <v>6.27</v>
       </c>
       <c r="J14" s="6">
-        <v>28.979999999999997</v>
+        <v>27.099999999999998</v>
       </c>
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
       <c r="M14" s="6"/>
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
-      <c r="P14" s="6"/>
-      <c r="Q14" s="5"/>
+      <c r="P14" s="5"/>
+      <c r="Q14" s="6"/>
       <c r="R14" s="5"/>
-      <c r="S14" s="6"/>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="S14" s="5"/>
+      <c r="T14" s="5"/>
+      <c r="U14" s="6"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" t="str" cm="1">
         <f t="array" ref="A15">IF(C15="P",SUMPRODUCT(--(D$3:D$82&gt;D15),--(C$3:C$82="P"))+1,"")</f>
         <v/>
       </c>
       <c r="B15" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="5">
-        <f t="shared" si="0"/>
-        <v>70.900000000000006</v>
+        <f>SUM(E15:G15)</f>
+        <v>79.69</v>
       </c>
       <c r="E15" s="5">
-        <f t="shared" si="1"/>
-        <v>49.97</v>
+        <f>MAX(H15:M15)</f>
+        <v>50.71</v>
       </c>
       <c r="F15" s="5">
-        <f t="shared" si="2"/>
-        <v>20.93</v>
+        <f>IF(COUNT(H15:M15)&gt;1,LARGE(H15:M15,2),0)</f>
+        <v>28.979999999999997</v>
       </c>
       <c r="G15" s="6">
-        <f t="shared" si="3"/>
+        <f>IF(MAX(N15:U15)-F15&gt;0,MAX(N15:U15)-F15,0)</f>
         <v>0</v>
       </c>
       <c r="H15" s="5">
-        <v>49.97</v>
+        <v>50.71</v>
       </c>
       <c r="I15" s="5">
-        <v>20.93</v>
+        <v>17.73</v>
       </c>
       <c r="J15" s="6">
-        <v>5.7299999999999995</v>
+        <v>28.979999999999997</v>
       </c>
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
       <c r="M15" s="6"/>
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
-      <c r="P15" s="6"/>
-      <c r="Q15" s="5"/>
+      <c r="P15" s="5"/>
+      <c r="Q15" s="6"/>
       <c r="R15" s="5"/>
-      <c r="S15" s="6"/>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="S15" s="5"/>
+      <c r="T15" s="5"/>
+      <c r="U15" s="6"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" t="str" cm="1">
         <f t="array" ref="A16">IF(C16="P",SUMPRODUCT(--(D$3:D$82&gt;D16),--(C$3:C$82="P"))+1,"")</f>
         <v/>
       </c>
       <c r="B16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="5">
-        <f t="shared" si="0"/>
-        <v>58.769999999999996</v>
+        <f>SUM(E16:G16)</f>
+        <v>70.900000000000006</v>
       </c>
       <c r="E16" s="5">
-        <f t="shared" si="1"/>
-        <v>30.43</v>
+        <f>MAX(H16:M16)</f>
+        <v>49.97</v>
       </c>
       <c r="F16" s="5">
-        <f t="shared" si="2"/>
-        <v>28.34</v>
+        <f>IF(COUNT(H16:M16)&gt;1,LARGE(H16:M16,2),0)</f>
+        <v>20.93</v>
       </c>
       <c r="G16" s="6">
-        <f t="shared" si="3"/>
+        <f>IF(MAX(N16:U16)-F16&gt;0,MAX(N16:U16)-F16,0)</f>
         <v>0</v>
       </c>
       <c r="H16" s="5">
-        <v>30.43</v>
+        <v>49.97</v>
       </c>
       <c r="I16" s="5">
-        <v>28.34</v>
-      </c>
-      <c r="J16" s="6"/>
+        <v>20.93</v>
+      </c>
+      <c r="J16" s="6">
+        <v>5.7299999999999995</v>
+      </c>
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
       <c r="M16" s="6"/>
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
-      <c r="P16" s="6"/>
-      <c r="Q16" s="5"/>
+      <c r="P16" s="5"/>
+      <c r="Q16" s="6"/>
       <c r="R16" s="5"/>
-      <c r="S16" s="6"/>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="S16" s="5"/>
+      <c r="T16" s="5"/>
+      <c r="U16" s="6"/>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A17" t="str" cm="1">
         <f t="array" ref="A17">IF(C17="P",SUMPRODUCT(--(D$3:D$82&gt;D17),--(C$3:C$82="P"))+1,"")</f>
         <v/>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="5">
-        <f t="shared" si="0"/>
-        <v>54.26</v>
+        <f>SUM(E17:G17)</f>
+        <v>58.769999999999996</v>
       </c>
       <c r="E17" s="5">
-        <f t="shared" si="1"/>
-        <v>43.16</v>
+        <f>MAX(H17:M17)</f>
+        <v>30.43</v>
       </c>
       <c r="F17" s="5">
-        <f t="shared" si="2"/>
-        <v>11.1</v>
+        <f>IF(COUNT(H17:M17)&gt;1,LARGE(H17:M17,2),0)</f>
+        <v>28.34</v>
       </c>
       <c r="G17" s="6">
-        <f t="shared" si="3"/>
+        <f>IF(MAX(N17:U17)-F17&gt;0,MAX(N17:U17)-F17,0)</f>
         <v>0</v>
       </c>
       <c r="H17" s="5">
-        <v>43.16</v>
+        <v>30.43</v>
       </c>
       <c r="I17" s="5">
-        <v>11.1</v>
+        <v>28.34</v>
       </c>
       <c r="J17" s="6"/>
       <c r="K17" s="5"/>
@@ -1404,43 +1494,43 @@
       <c r="M17" s="6"/>
       <c r="N17" s="5"/>
       <c r="O17" s="5"/>
-      <c r="P17" s="6"/>
-      <c r="Q17" s="5"/>
+      <c r="P17" s="5"/>
+      <c r="Q17" s="6"/>
       <c r="R17" s="5"/>
-      <c r="S17" s="6"/>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A18" cm="1">
+      <c r="S17" s="5"/>
+      <c r="T17" s="5"/>
+      <c r="U17" s="6"/>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A18" t="str" cm="1">
         <f t="array" ref="A18">IF(C18="P",SUMPRODUCT(--(D$3:D$82&gt;D18),--(C$3:C$82="P"))+1,"")</f>
-        <v>6</v>
+        <v/>
       </c>
       <c r="B18" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>4</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="C18" s="3"/>
       <c r="D18" s="5">
-        <f t="shared" si="0"/>
-        <v>42.17</v>
+        <f>SUM(E18:G18)</f>
+        <v>54.26</v>
       </c>
       <c r="E18" s="5">
-        <f t="shared" si="1"/>
-        <v>35.85</v>
+        <f>MAX(H18:M18)</f>
+        <v>43.16</v>
       </c>
       <c r="F18" s="5">
-        <f t="shared" si="2"/>
-        <v>6.3199999999999994</v>
+        <f>IF(COUNT(H18:M18)&gt;1,LARGE(H18:M18,2),0)</f>
+        <v>11.1</v>
       </c>
       <c r="G18" s="6">
-        <f t="shared" si="3"/>
+        <f>IF(MAX(N18:U18)-F18&gt;0,MAX(N18:U18)-F18,0)</f>
         <v>0</v>
       </c>
       <c r="H18" s="5">
-        <v>6.3199999999999994</v>
+        <v>43.16</v>
       </c>
       <c r="I18" s="5">
-        <v>35.85</v>
+        <v>11.1</v>
       </c>
       <c r="J18" s="6"/>
       <c r="K18" s="5"/>
@@ -1448,12 +1538,14 @@
       <c r="M18" s="6"/>
       <c r="N18" s="5"/>
       <c r="O18" s="5"/>
-      <c r="P18" s="6"/>
-      <c r="Q18" s="5"/>
+      <c r="P18" s="5"/>
+      <c r="Q18" s="6"/>
       <c r="R18" s="5"/>
-      <c r="S18" s="6"/>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="S18" s="5"/>
+      <c r="T18" s="5"/>
+      <c r="U18" s="6"/>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A19" t="str" cm="1">
         <f t="array" ref="A19">IF(C19="P",SUMPRODUCT(--(D$3:D$82&gt;D19),--(C$3:C$82="P"))+1,"")</f>
         <v/>
@@ -1463,19 +1555,19 @@
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="5">
-        <f t="shared" si="0"/>
+        <f>SUM(E19:G19)</f>
         <v>37.99</v>
       </c>
       <c r="E19" s="5">
-        <f t="shared" si="1"/>
+        <f>MAX(H19:M19)</f>
         <v>21.73</v>
       </c>
       <c r="F19" s="5">
-        <f t="shared" si="2"/>
+        <f>IF(COUNT(H19:M19)&gt;1,LARGE(H19:M19,2),0)</f>
         <v>16.260000000000002</v>
       </c>
       <c r="G19" s="6">
-        <f t="shared" si="3"/>
+        <f>IF(MAX(N19:U19)-F19&gt;0,MAX(N19:U19)-F19,0)</f>
         <v>0</v>
       </c>
       <c r="H19" s="5">
@@ -1490,37 +1582,41 @@
       <c r="M19" s="6"/>
       <c r="N19" s="5"/>
       <c r="O19" s="5"/>
-      <c r="P19" s="6"/>
-      <c r="Q19" s="5"/>
+      <c r="P19" s="5"/>
+      <c r="Q19" s="6"/>
       <c r="R19" s="5"/>
-      <c r="S19" s="6"/>
+      <c r="S19" s="5"/>
+      <c r="T19" s="5"/>
+      <c r="U19" s="6"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:T2" xr:uid="{58EF7559-DEC1-374C-BE9A-EB931A8A53CD}">
+  <autoFilter ref="A1:V2" xr:uid="{58EF7559-DEC1-374C-BE9A-EB931A8A53CD}">
     <filterColumn colId="7" showButton="0"/>
     <filterColumn colId="8" showButton="0"/>
     <filterColumn colId="10" showButton="0"/>
     <filterColumn colId="11" showButton="0"/>
     <filterColumn colId="13" showButton="0"/>
     <filterColumn colId="14" showButton="0"/>
-    <filterColumn colId="16" showButton="0"/>
+    <filterColumn colId="15" showButton="0"/>
     <filterColumn colId="17" showButton="0"/>
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:T19">
+    <filterColumn colId="18" showButton="0"/>
+    <filterColumn colId="19" showButton="0"/>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:U19">
       <sortCondition descending="1" ref="D1:D19"/>
     </sortState>
   </autoFilter>
   <mergeCells count="11">
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="K1:M1"/>
-    <mergeCell ref="N1:P1"/>
-    <mergeCell ref="Q1:S1"/>
-    <mergeCell ref="G1:G2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="R1:U1"/>
+    <mergeCell ref="G1:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1528,7 +1624,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8E6522B-64E0-3048-88A5-2C33C62E09E6}">
-  <dimension ref="A1:S7"/>
+  <dimension ref="A1:U7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:A2"/>
@@ -1541,61 +1637,63 @@
     <col min="7" max="7" width="15.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.83203125" style="4"/>
     <col min="13" max="13" width="10.83203125" style="4"/>
-    <col min="16" max="16" width="10.83203125" style="4"/>
-    <col min="19" max="19" width="10.83203125" style="4"/>
+    <col min="17" max="17" width="10.83203125" style="4"/>
+    <col min="21" max="21" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="14"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="13" t="s">
+      <c r="I1" s="8"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="14"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="13" t="s">
+      <c r="L1" s="8"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="14"/>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="R1" s="14"/>
-      <c r="S1" s="15"/>
-    </row>
-    <row r="2" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="10"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="9"/>
+    </row>
+    <row r="2" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="13"/>
       <c r="H2" s="1" t="s">
         <v>9</v>
       </c>
@@ -1620,20 +1718,26 @@
       <c r="O2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="P2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="T2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="U2" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A3" cm="1">
         <f t="array" ref="A3">IF(C3="P",SUMPRODUCT(--(D$3:D$55&gt;D3),--(C$3:C$55="P"))+1,"")</f>
         <v>1</v>
@@ -1657,7 +1761,7 @@
         <v>51.46</v>
       </c>
       <c r="G3" s="6">
-        <f>IF(MAX(N3:S3)-F3&gt;0,MAX(N3:S3)-F3,0)</f>
+        <f>IF(MAX(N3:U3)-F3&gt;0,MAX(N3:U3)-F3,0)</f>
         <v>0</v>
       </c>
       <c r="H3" s="5">
@@ -1674,12 +1778,14 @@
       <c r="M3" s="6"/>
       <c r="N3" s="5"/>
       <c r="O3" s="5"/>
-      <c r="P3" s="6"/>
-      <c r="Q3" s="5"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="6"/>
       <c r="R3" s="5"/>
-      <c r="S3" s="6"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="S3" s="5"/>
+      <c r="T3" s="5"/>
+      <c r="U3" s="6"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" cm="1">
         <f t="array" ref="A4">IF(C4="P",SUMPRODUCT(--(D$3:D$55&gt;D4),--(C$3:C$55="P"))+1,"")</f>
         <v>2</v>
@@ -1692,7 +1798,7 @@
       </c>
       <c r="D4" s="5">
         <f>SUM(E4:G4)</f>
-        <v>102.04</v>
+        <v>102.82000000000001</v>
       </c>
       <c r="E4" s="5">
         <f>MAX(H4:M4)</f>
@@ -1703,8 +1809,8 @@
         <v>50.89</v>
       </c>
       <c r="G4" s="6">
-        <f>IF(MAX(N4:S4)-F4&gt;0,MAX(N4:S4)-F4,0)</f>
-        <v>0</v>
+        <f>IF(MAX(N4:U4)-F4&gt;0,MAX(N4:U4)-F4,0)</f>
+        <v>0.78000000000000114</v>
       </c>
       <c r="H4" s="5">
         <v>51.150000000000006</v>
@@ -1718,14 +1824,22 @@
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
       <c r="M4" s="6"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
-      <c r="P4" s="6"/>
-      <c r="Q4" s="5"/>
+      <c r="N4" s="5">
+        <v>50.39</v>
+      </c>
+      <c r="O4" s="5">
+        <v>51.67</v>
+      </c>
+      <c r="P4" s="5">
+        <v>50.79</v>
+      </c>
+      <c r="Q4" s="6"/>
       <c r="R4" s="5"/>
-      <c r="S4" s="6"/>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="S4" s="5"/>
+      <c r="T4" s="5"/>
+      <c r="U4" s="6"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" cm="1">
         <f t="array" ref="A5">IF(C5="P",SUMPRODUCT(--(D$3:D$55&gt;D5),--(C$3:C$55="P"))+1,"")</f>
         <v>3</v>
@@ -1749,7 +1863,7 @@
         <v>47.769999999999996</v>
       </c>
       <c r="G5" s="6">
-        <f>IF(MAX(N5:S5)-F5&gt;0,MAX(N5:S5)-F5,0)</f>
+        <f>IF(MAX(N5:U5)-F5&gt;0,MAX(N5:U5)-F5,0)</f>
         <v>0</v>
       </c>
       <c r="H5" s="5">
@@ -1766,12 +1880,14 @@
       <c r="M5" s="6"/>
       <c r="N5" s="5"/>
       <c r="O5" s="5"/>
-      <c r="P5" s="6"/>
-      <c r="Q5" s="5"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="6"/>
       <c r="R5" s="5"/>
-      <c r="S5" s="6"/>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="S5" s="5"/>
+      <c r="T5" s="5"/>
+      <c r="U5" s="6"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" t="str" cm="1">
         <f t="array" ref="A6">IF(C6="P",SUMPRODUCT(--(D$3:D$55&gt;D6),--(C$3:C$55="P"))+1,"")</f>
         <v/>
@@ -1792,7 +1908,7 @@
         <v>41.37</v>
       </c>
       <c r="G6" s="6">
-        <f>IF(MAX(N6:S6)-F6&gt;0,MAX(N6:S6)-F6,0)</f>
+        <f>IF(MAX(N6:U6)-F6&gt;0,MAX(N6:U6)-F6,0)</f>
         <v>0</v>
       </c>
       <c r="H6" s="5">
@@ -1809,12 +1925,14 @@
       <c r="M6" s="6"/>
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
-      <c r="P6" s="6"/>
-      <c r="Q6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="6"/>
       <c r="R6" s="5"/>
-      <c r="S6" s="6"/>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="S6" s="5"/>
+      <c r="T6" s="5"/>
+      <c r="U6" s="6"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" cm="1">
         <f t="array" ref="A7">IF(C7="P",SUMPRODUCT(--(D$3:D$55&gt;D7),--(C$3:C$55="P"))+1,"")</f>
         <v>4</v>
@@ -1838,7 +1956,7 @@
         <v>25.22</v>
       </c>
       <c r="G7" s="6">
-        <f>IF(MAX(N7:S7)-F7&gt;0,MAX(N7:S7)-F7,0)</f>
+        <f>IF(MAX(N7:U7)-F7&gt;0,MAX(N7:U7)-F7,0)</f>
         <v>0</v>
       </c>
       <c r="H7" s="5">
@@ -1855,37 +1973,41 @@
       <c r="M7" s="6"/>
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
-      <c r="P7" s="6"/>
-      <c r="Q7" s="5"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="6"/>
       <c r="R7" s="5"/>
-      <c r="S7" s="6"/>
+      <c r="S7" s="5"/>
+      <c r="T7" s="5"/>
+      <c r="U7" s="6"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:T2" xr:uid="{58EF7559-DEC1-374C-BE9A-EB931A8A53CD}">
+  <autoFilter ref="A1:V2" xr:uid="{58EF7559-DEC1-374C-BE9A-EB931A8A53CD}">
     <filterColumn colId="7" showButton="0"/>
     <filterColumn colId="8" showButton="0"/>
     <filterColumn colId="10" showButton="0"/>
     <filterColumn colId="11" showButton="0"/>
     <filterColumn colId="13" showButton="0"/>
     <filterColumn colId="14" showButton="0"/>
-    <filterColumn colId="16" showButton="0"/>
+    <filterColumn colId="15" showButton="0"/>
     <filterColumn colId="17" showButton="0"/>
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:S7">
+    <filterColumn colId="18" showButton="0"/>
+    <filterColumn colId="19" showButton="0"/>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:U7">
       <sortCondition descending="1" ref="D1:D7"/>
     </sortState>
   </autoFilter>
   <mergeCells count="11">
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="R1:U1"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="K1:M1"/>
-    <mergeCell ref="N1:P1"/>
-    <mergeCell ref="Q1:S1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>